<commit_message>
Correct species name and remove aberrant data
</commit_message>
<xml_diff>
--- a/data/villefranche/catches.xlsx
+++ b/data/villefranche/catches.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="125725" refMode="R1C1" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9306" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9305" uniqueCount="963">
   <si>
     <t>gear</t>
   </si>
@@ -10643,7 +10643,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B79" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -11289,7 +11289,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L152" sqref="L152"/>
+      <selection pane="bottomRight" activeCell="F1489" sqref="F1489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15179,7 +15179,7 @@
         <v>807</v>
       </c>
       <c r="F155" t="s">
-        <v>865</v>
+        <v>847</v>
       </c>
       <c r="G155" t="s">
         <v>10</v>
@@ -15249,7 +15249,7 @@
         <v>807</v>
       </c>
       <c r="F158" t="s">
-        <v>865</v>
+        <v>847</v>
       </c>
       <c r="G158" t="s">
         <v>10</v>
@@ -15353,9 +15353,7 @@
       <c r="D162" t="s">
         <v>133</v>
       </c>
-      <c r="F162" t="s">
-        <v>865</v>
-      </c>
+      <c r="F162"/>
       <c r="G162" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fix a catch at 0 which was actually identified
</commit_message>
<xml_diff>
--- a/data/villefranche/catches.xlsx
+++ b/data/villefranche/catches.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/fish/radeichthyo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiho/Work/projects/medplanet/data/villefranche/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,9 +23,6 @@
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -3037,14 +3034,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11286,10 +11283,10 @@
   <dimension ref="A1:L1615"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D758" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1489" sqref="F1489"/>
+      <selection pane="bottomRight" activeCell="H805" sqref="H805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33353,7 +33350,7 @@
         <v>10</v>
       </c>
       <c r="H805">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L805" t="s">
         <v>530</v>

</xml_diff>

<commit_message>
Remove warnings and errors in data preparation
</commit_message>
<xml_diff>
--- a/data/villefranche/catches.xlsx
+++ b/data/villefranche/catches.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiho/Work/projects/medplanet/data/villefranche/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiho/Library/Caches/Transmit/BF8722BA-40CB-4602-A8A5-871C4D5D471E/niko.obs-vlfr.fr/home/jiho/gdrive/projects/medplanet/data/villefranche/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9305" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9303" uniqueCount="961">
   <si>
     <t>gear</t>
   </si>
@@ -2748,9 +2748,6 @@
     <t>Just the head. Unidentifiable</t>
   </si>
   <si>
-    <t>&gt;100</t>
-  </si>
-  <si>
     <t>Sparidae?</t>
   </si>
   <si>
@@ -2758,9 +2755,6 @@
   </si>
   <si>
     <t>species_suffix</t>
-  </si>
-  <si>
-    <t>~10</t>
   </si>
   <si>
     <t>Big one adult squid in CARE</t>
@@ -11283,10 +11277,10 @@
   <dimension ref="A1:L1615"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D758" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D1481" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H805" sqref="H805"/>
+      <selection pane="bottomRight" activeCell="I1508" sqref="I1508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11322,7 +11316,7 @@
         <v>804</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -11331,7 +11325,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>803</v>
@@ -11369,7 +11363,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="J2" t="s">
         <v>799</v>
@@ -11454,7 +11448,7 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -13856,7 +13850,7 @@
         <v>1</v>
       </c>
       <c r="L102" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
@@ -42165,7 +42159,7 @@
         <v>1</v>
       </c>
       <c r="L1155" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1156" spans="1:12" x14ac:dyDescent="0.2">
@@ -42252,7 +42246,7 @@
         <v>6</v>
       </c>
       <c r="L1158" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1159" spans="1:12" x14ac:dyDescent="0.2">
@@ -49943,19 +49937,19 @@
         <v>97</v>
       </c>
       <c r="E1473" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="F1473" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H1473">
         <v>1</v>
       </c>
       <c r="I1473" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1473" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="1474" spans="1:12" x14ac:dyDescent="0.2">
@@ -49996,7 +49990,7 @@
         <v>1</v>
       </c>
       <c r="I1475" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1476" spans="1:12" x14ac:dyDescent="0.2">
@@ -50118,14 +50112,14 @@
         <v>7</v>
       </c>
       <c r="D1483" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="F1483"/>
       <c r="H1483">
         <v>1</v>
       </c>
       <c r="I1483" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1483" t="s">
         <v>793</v>
@@ -50148,13 +50142,13 @@
         <v>814</v>
       </c>
       <c r="F1484" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="H1484">
         <v>1</v>
       </c>
       <c r="I1484" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1484" t="s">
         <v>793</v>
@@ -50183,7 +50177,7 @@
         <v>2</v>
       </c>
       <c r="I1485" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1485" t="s">
         <v>793</v>
@@ -50227,7 +50221,7 @@
         <v>1</v>
       </c>
       <c r="I1487" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1488" spans="1:12" x14ac:dyDescent="0.2">
@@ -50244,7 +50238,7 @@
         <v>25</v>
       </c>
       <c r="E1488" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1488" t="s">
         <v>873</v>
@@ -50253,7 +50247,7 @@
         <v>3</v>
       </c>
       <c r="I1488" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1489" spans="1:9" x14ac:dyDescent="0.2">
@@ -50279,7 +50273,7 @@
         <v>1</v>
       </c>
       <c r="I1489" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1490" spans="1:9" x14ac:dyDescent="0.2">
@@ -50296,7 +50290,7 @@
         <v>25</v>
       </c>
       <c r="E1490" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1490" t="s">
         <v>873</v>
@@ -50305,7 +50299,7 @@
         <v>1</v>
       </c>
       <c r="I1490" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1491" spans="1:9" x14ac:dyDescent="0.2">
@@ -50331,7 +50325,7 @@
         <v>6</v>
       </c>
       <c r="I1491" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1492" spans="1:9" x14ac:dyDescent="0.2">
@@ -50357,7 +50351,7 @@
         <v>7</v>
       </c>
       <c r="I1492" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1493" spans="1:9" x14ac:dyDescent="0.2">
@@ -50383,7 +50377,7 @@
         <v>1</v>
       </c>
       <c r="I1493" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1494" spans="1:9" x14ac:dyDescent="0.2">
@@ -50409,7 +50403,7 @@
         <v>3</v>
       </c>
       <c r="I1494" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1495" spans="1:9" x14ac:dyDescent="0.2">
@@ -50435,7 +50429,7 @@
         <v>5</v>
       </c>
       <c r="I1495" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1496" spans="1:9" x14ac:dyDescent="0.2">
@@ -50452,7 +50446,7 @@
         <v>25</v>
       </c>
       <c r="E1496" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1496" s="2" t="s">
         <v>873</v>
@@ -50461,7 +50455,7 @@
         <v>2</v>
       </c>
       <c r="I1496" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1497" spans="1:9" x14ac:dyDescent="0.2">
@@ -50478,7 +50472,7 @@
         <v>25</v>
       </c>
       <c r="E1497" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1497" s="2" t="s">
         <v>873</v>
@@ -50487,7 +50481,7 @@
         <v>2</v>
       </c>
       <c r="I1497" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1498" spans="1:9" x14ac:dyDescent="0.2">
@@ -50504,7 +50498,7 @@
         <v>25</v>
       </c>
       <c r="E1498" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1498" s="2" t="s">
         <v>873</v>
@@ -50513,7 +50507,7 @@
         <v>1</v>
       </c>
       <c r="I1498" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1499" spans="1:9" x14ac:dyDescent="0.2">
@@ -50539,7 +50533,7 @@
         <v>2</v>
       </c>
       <c r="I1499" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1500" spans="1:9" x14ac:dyDescent="0.2">
@@ -50553,10 +50547,10 @@
         <v>7</v>
       </c>
       <c r="D1500" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E1500" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1500" s="2" t="s">
         <v>873</v>
@@ -50565,7 +50559,7 @@
         <v>1</v>
       </c>
       <c r="I1500" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1501" spans="1:9" x14ac:dyDescent="0.2">
@@ -50591,7 +50585,7 @@
         <v>12</v>
       </c>
       <c r="I1501" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1502" spans="1:9" x14ac:dyDescent="0.2">
@@ -50617,7 +50611,7 @@
         <v>8</v>
       </c>
       <c r="I1502" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1503" spans="1:9" x14ac:dyDescent="0.2">
@@ -50634,7 +50628,7 @@
         <v>25</v>
       </c>
       <c r="E1503" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1503" s="2" t="s">
         <v>873</v>
@@ -50643,7 +50637,7 @@
         <v>1</v>
       </c>
       <c r="I1503" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1504" spans="1:9" x14ac:dyDescent="0.2">
@@ -50657,14 +50651,14 @@
         <v>7</v>
       </c>
       <c r="D1504" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E1504" s="7"/>
       <c r="H1504">
         <v>1</v>
       </c>
       <c r="I1504" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1505" spans="1:12" x14ac:dyDescent="0.2">
@@ -50681,7 +50675,7 @@
         <v>25</v>
       </c>
       <c r="E1505" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1505" s="2" t="s">
         <v>873</v>
@@ -50690,7 +50684,7 @@
         <v>1</v>
       </c>
       <c r="I1505" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1506" spans="1:12" x14ac:dyDescent="0.2">
@@ -50704,17 +50698,17 @@
         <v>7</v>
       </c>
       <c r="D1506" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E1506" s="7"/>
       <c r="H1506">
         <v>2</v>
       </c>
       <c r="I1506" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1506" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="1507" spans="1:12" x14ac:dyDescent="0.2">
@@ -50728,13 +50722,13 @@
         <v>7</v>
       </c>
       <c r="D1507" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="H1507">
         <v>1</v>
       </c>
       <c r="I1507" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1508" spans="1:12" x14ac:dyDescent="0.2">
@@ -50745,10 +50739,10 @@
         <v>7</v>
       </c>
       <c r="D1508" t="s">
-        <v>907</v>
-      </c>
-      <c r="H1508" t="s">
-        <v>905</v>
+        <v>906</v>
+      </c>
+      <c r="H1508">
+        <v>100</v>
       </c>
     </row>
     <row r="1509" spans="1:12" x14ac:dyDescent="0.2">
@@ -50774,7 +50768,7 @@
         <v>10</v>
       </c>
       <c r="I1509" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1510" spans="1:12" x14ac:dyDescent="0.2">
@@ -50800,7 +50794,7 @@
         <v>3</v>
       </c>
       <c r="I1510" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1511" spans="1:12" x14ac:dyDescent="0.2">
@@ -50826,7 +50820,7 @@
         <v>1</v>
       </c>
       <c r="I1511" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1512" spans="1:12" x14ac:dyDescent="0.2">
@@ -50840,16 +50834,16 @@
         <v>7</v>
       </c>
       <c r="D1512" t="s">
+        <v>929</v>
+      </c>
+      <c r="H1512">
+        <v>1</v>
+      </c>
+      <c r="I1512" t="s">
+        <v>910</v>
+      </c>
+      <c r="L1512" t="s">
         <v>931</v>
-      </c>
-      <c r="H1512">
-        <v>1</v>
-      </c>
-      <c r="I1512" t="s">
-        <v>912</v>
-      </c>
-      <c r="L1512" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="1513" spans="1:12" x14ac:dyDescent="0.2">
@@ -50866,7 +50860,7 @@
         <v>25</v>
       </c>
       <c r="E1513" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F1513" s="2" t="s">
         <v>873</v>
@@ -50875,7 +50869,7 @@
         <v>1</v>
       </c>
       <c r="I1513" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1514" spans="1:12" x14ac:dyDescent="0.2">
@@ -50896,7 +50890,7 @@
         <v>1</v>
       </c>
       <c r="I1514" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1515" spans="1:12" x14ac:dyDescent="0.2">
@@ -50922,10 +50916,10 @@
         <v>1</v>
       </c>
       <c r="I1515" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1515" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="1516" spans="1:12" x14ac:dyDescent="0.2">
@@ -50951,7 +50945,7 @@
         <v>3</v>
       </c>
       <c r="I1516" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1517" spans="1:12" x14ac:dyDescent="0.2">
@@ -50977,7 +50971,7 @@
         <v>4</v>
       </c>
       <c r="I1517" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1518" spans="1:12" x14ac:dyDescent="0.2">
@@ -51003,10 +50997,10 @@
         <v>1</v>
       </c>
       <c r="I1518" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1518" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="1519" spans="1:12" x14ac:dyDescent="0.2">
@@ -51020,7 +51014,7 @@
         <v>7</v>
       </c>
       <c r="D1519" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E1519" t="s">
         <v>843</v>
@@ -51035,7 +51029,7 @@
         <v>1</v>
       </c>
       <c r="I1519" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1520" spans="1:12" x14ac:dyDescent="0.2">
@@ -51061,7 +51055,7 @@
         <v>1</v>
       </c>
       <c r="I1520" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1521" spans="1:12" x14ac:dyDescent="0.2">
@@ -51075,10 +51069,10 @@
         <v>7</v>
       </c>
       <c r="D1521" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E1521" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="F1521" s="2" t="s">
         <v>861</v>
@@ -51087,7 +51081,7 @@
         <v>1</v>
       </c>
       <c r="I1521" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1522" spans="1:12" x14ac:dyDescent="0.2">
@@ -51104,7 +51098,7 @@
         <v>8</v>
       </c>
       <c r="E1522" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F1522" s="2" t="s">
         <v>877</v>
@@ -51113,7 +51107,7 @@
         <v>1</v>
       </c>
       <c r="I1522" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1523" spans="1:12" x14ac:dyDescent="0.2">
@@ -51133,10 +51127,10 @@
         <v>1</v>
       </c>
       <c r="I1523" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1523" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="1524" spans="1:12" x14ac:dyDescent="0.2">
@@ -51162,10 +51156,10 @@
         <v>1</v>
       </c>
       <c r="I1524" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1524" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="1525" spans="1:12" x14ac:dyDescent="0.2">
@@ -51191,7 +51185,7 @@
         <v>1</v>
       </c>
       <c r="I1525" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1526" spans="1:12" x14ac:dyDescent="0.2">
@@ -51211,10 +51205,10 @@
         <v>1</v>
       </c>
       <c r="I1526" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1526" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="1527" spans="1:12" x14ac:dyDescent="0.2">
@@ -51240,7 +51234,7 @@
         <v>1</v>
       </c>
       <c r="I1527" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1528" spans="1:12" x14ac:dyDescent="0.2">
@@ -51266,7 +51260,7 @@
         <v>1</v>
       </c>
       <c r="I1528" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="1529" spans="1:12" x14ac:dyDescent="0.2">
@@ -51292,7 +51286,7 @@
         <v>2</v>
       </c>
       <c r="I1529" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1530" spans="1:12" x14ac:dyDescent="0.2">
@@ -51318,7 +51312,7 @@
         <v>1</v>
       </c>
       <c r="I1530" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1531" spans="1:12" x14ac:dyDescent="0.2">
@@ -51332,7 +51326,7 @@
         <v>7</v>
       </c>
       <c r="D1531" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H1531">
         <v>30</v>
@@ -51361,7 +51355,7 @@
         <v>1</v>
       </c>
       <c r="I1532" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1533" spans="1:12" x14ac:dyDescent="0.2">
@@ -51387,7 +51381,7 @@
         <v>1</v>
       </c>
       <c r="I1533" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1534" spans="1:12" x14ac:dyDescent="0.2">
@@ -51413,7 +51407,7 @@
         <v>2</v>
       </c>
       <c r="I1534" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1535" spans="1:12" x14ac:dyDescent="0.2">
@@ -51439,7 +51433,7 @@
         <v>7</v>
       </c>
       <c r="I1535" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1536" spans="1:12" x14ac:dyDescent="0.2">
@@ -51465,7 +51459,7 @@
         <v>5</v>
       </c>
       <c r="I1536" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1537" spans="1:12" x14ac:dyDescent="0.2">
@@ -51485,13 +51479,13 @@
         <v>806</v>
       </c>
       <c r="F1537" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H1537">
         <v>1</v>
       </c>
       <c r="I1537" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1538" spans="1:12" x14ac:dyDescent="0.2">
@@ -51517,7 +51511,7 @@
         <v>5</v>
       </c>
       <c r="I1538" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1539" spans="1:12" x14ac:dyDescent="0.2">
@@ -51543,7 +51537,7 @@
         <v>1</v>
       </c>
       <c r="I1539" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1540" spans="1:12" x14ac:dyDescent="0.2">
@@ -51569,7 +51563,7 @@
         <v>1</v>
       </c>
       <c r="I1540" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1541" spans="1:12" x14ac:dyDescent="0.2">
@@ -51583,7 +51577,7 @@
         <v>7</v>
       </c>
       <c r="D1541" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="1542" spans="1:12" x14ac:dyDescent="0.2">
@@ -51599,8 +51593,8 @@
       <c r="D1542" t="s">
         <v>792</v>
       </c>
-      <c r="H1542" t="s">
-        <v>909</v>
+      <c r="H1542">
+        <v>10</v>
       </c>
     </row>
     <row r="1543" spans="1:12" x14ac:dyDescent="0.2">
@@ -51649,7 +51643,7 @@
         <v>4</v>
       </c>
       <c r="I1544" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1545" spans="1:12" x14ac:dyDescent="0.2">
@@ -51675,10 +51669,10 @@
         <v>1</v>
       </c>
       <c r="I1545" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1545" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="1546" spans="1:12" x14ac:dyDescent="0.2">
@@ -51704,7 +51698,7 @@
         <v>1</v>
       </c>
       <c r="I1546" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1547" spans="1:12" x14ac:dyDescent="0.2">
@@ -51730,7 +51724,7 @@
         <v>41</v>
       </c>
       <c r="I1547" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1548" spans="1:12" x14ac:dyDescent="0.2">
@@ -51756,7 +51750,7 @@
         <v>4</v>
       </c>
       <c r="I1548" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1549" spans="1:12" x14ac:dyDescent="0.2">
@@ -51782,7 +51776,7 @@
         <v>15</v>
       </c>
       <c r="I1549" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1550" spans="1:12" x14ac:dyDescent="0.2">
@@ -51808,7 +51802,7 @@
         <v>2</v>
       </c>
       <c r="I1550" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1551" spans="1:12" x14ac:dyDescent="0.2">
@@ -51828,13 +51822,13 @@
         <v>806</v>
       </c>
       <c r="F1551" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H1551">
         <v>3</v>
       </c>
       <c r="I1551" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1552" spans="1:12" x14ac:dyDescent="0.2">
@@ -51860,7 +51854,7 @@
         <v>4</v>
       </c>
       <c r="I1552" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1553" spans="1:12" x14ac:dyDescent="0.2">
@@ -51880,13 +51874,13 @@
         <v>806</v>
       </c>
       <c r="F1553" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H1553">
         <v>1</v>
       </c>
       <c r="I1553" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1554" spans="1:12" x14ac:dyDescent="0.2">
@@ -51912,7 +51906,7 @@
         <v>2</v>
       </c>
       <c r="I1554" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1555" spans="1:12" x14ac:dyDescent="0.2">
@@ -51932,7 +51926,7 @@
         <v>3</v>
       </c>
       <c r="I1555" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1556" spans="1:12" x14ac:dyDescent="0.2">
@@ -51958,7 +51952,7 @@
         <v>1</v>
       </c>
       <c r="I1556" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1557" spans="1:12" x14ac:dyDescent="0.2">
@@ -51998,7 +51992,7 @@
         <v>1</v>
       </c>
       <c r="I1558" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1559" spans="1:12" x14ac:dyDescent="0.2">
@@ -52038,7 +52032,7 @@
         <v>1</v>
       </c>
       <c r="I1560" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1561" spans="1:12" x14ac:dyDescent="0.2">
@@ -52061,7 +52055,7 @@
         <v>15</v>
       </c>
       <c r="I1561" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1562" spans="1:12" x14ac:dyDescent="0.2">
@@ -52087,10 +52081,10 @@
         <v>1</v>
       </c>
       <c r="I1562" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1562" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="1563" spans="1:12" x14ac:dyDescent="0.2">
@@ -52110,16 +52104,16 @@
         <v>806</v>
       </c>
       <c r="F1563" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H1563">
         <v>4</v>
       </c>
       <c r="I1563" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1563" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="1564" spans="1:12" x14ac:dyDescent="0.2">
@@ -52159,7 +52153,7 @@
         <v>8</v>
       </c>
       <c r="I1565" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="1566" spans="1:12" x14ac:dyDescent="0.2">
@@ -52185,7 +52179,7 @@
         <v>6</v>
       </c>
       <c r="I1566" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="1567" spans="1:12" x14ac:dyDescent="0.2">
@@ -52211,7 +52205,7 @@
         <v>16</v>
       </c>
       <c r="I1567" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="1568" spans="1:12" x14ac:dyDescent="0.2">
@@ -52237,10 +52231,10 @@
         <v>1</v>
       </c>
       <c r="I1568" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1568" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="1569" spans="1:12" x14ac:dyDescent="0.2">
@@ -52266,7 +52260,7 @@
         <v>1</v>
       </c>
       <c r="I1569" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1570" spans="1:12" x14ac:dyDescent="0.2">
@@ -52348,7 +52342,7 @@
         <v>4</v>
       </c>
       <c r="I1574" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1575" spans="1:12" x14ac:dyDescent="0.2">
@@ -52374,7 +52368,7 @@
         <v>1</v>
       </c>
       <c r="I1575" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1576" spans="1:12" x14ac:dyDescent="0.2">
@@ -52400,7 +52394,7 @@
         <v>2</v>
       </c>
       <c r="I1576" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1577" spans="1:12" x14ac:dyDescent="0.2">
@@ -52426,7 +52420,7 @@
         <v>2</v>
       </c>
       <c r="I1577" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1578" spans="1:12" x14ac:dyDescent="0.2">
@@ -52440,16 +52434,16 @@
         <v>7</v>
       </c>
       <c r="D1578" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="H1578">
         <v>1</v>
       </c>
       <c r="I1578" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1578" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="1579" spans="1:12" x14ac:dyDescent="0.2">
@@ -52475,7 +52469,7 @@
         <v>1</v>
       </c>
       <c r="I1579" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1580" spans="1:12" x14ac:dyDescent="0.2">
@@ -52501,7 +52495,7 @@
         <v>6</v>
       </c>
       <c r="I1580" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1581" spans="1:12" x14ac:dyDescent="0.2">
@@ -52527,7 +52521,7 @@
         <v>1</v>
       </c>
       <c r="I1581" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1582" spans="1:12" x14ac:dyDescent="0.2">
@@ -52553,7 +52547,7 @@
         <v>1</v>
       </c>
       <c r="I1582" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1583" spans="1:12" x14ac:dyDescent="0.2">
@@ -52579,7 +52573,7 @@
         <v>4</v>
       </c>
       <c r="I1583" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1584" spans="1:12" x14ac:dyDescent="0.2">
@@ -52599,16 +52593,16 @@
         <v>97</v>
       </c>
       <c r="F1584" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H1584">
         <v>3</v>
       </c>
       <c r="I1584" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1584" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="1585" spans="1:12" x14ac:dyDescent="0.2">
@@ -52622,10 +52616,10 @@
         <v>7</v>
       </c>
       <c r="D1585" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="E1585" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="F1585" s="2" t="s">
         <v>849</v>
@@ -52634,7 +52628,7 @@
         <v>4</v>
       </c>
       <c r="I1585" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1586" spans="1:12" x14ac:dyDescent="0.2">
@@ -52660,7 +52654,7 @@
         <v>1</v>
       </c>
       <c r="I1586" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1587" spans="1:12" x14ac:dyDescent="0.2">
@@ -52680,13 +52674,13 @@
         <v>97</v>
       </c>
       <c r="F1587" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H1587">
         <v>1</v>
       </c>
       <c r="I1587" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1588" spans="1:12" x14ac:dyDescent="0.2">
@@ -52712,7 +52706,7 @@
         <v>2</v>
       </c>
       <c r="I1588" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1589" spans="1:12" x14ac:dyDescent="0.2">
@@ -52732,10 +52726,10 @@
         <v>1</v>
       </c>
       <c r="I1589" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1589" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="1590" spans="1:12" x14ac:dyDescent="0.2">
@@ -52761,7 +52755,7 @@
         <v>1</v>
       </c>
       <c r="I1590" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1591" spans="1:12" x14ac:dyDescent="0.2">
@@ -52787,7 +52781,7 @@
         <v>3</v>
       </c>
       <c r="I1591" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1592" spans="1:12" x14ac:dyDescent="0.2">
@@ -52807,16 +52801,16 @@
         <v>805</v>
       </c>
       <c r="F1592" s="2" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="H1592">
         <v>1</v>
       </c>
       <c r="I1592" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1592" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="1593" spans="1:12" x14ac:dyDescent="0.2">
@@ -52842,7 +52836,7 @@
         <v>1</v>
       </c>
       <c r="I1593" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1594" spans="1:12" x14ac:dyDescent="0.2">
@@ -52862,13 +52856,13 @@
         <v>808</v>
       </c>
       <c r="F1594" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H1594">
         <v>1</v>
       </c>
       <c r="I1594" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1595" spans="1:12" x14ac:dyDescent="0.2">
@@ -52888,13 +52882,13 @@
         <v>822</v>
       </c>
       <c r="F1595" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H1595">
         <v>1</v>
       </c>
       <c r="I1595" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="1596" spans="1:12" x14ac:dyDescent="0.2">
@@ -52908,13 +52902,13 @@
         <v>7</v>
       </c>
       <c r="D1596" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1596" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F1596" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H1596">
         <v>2</v>
@@ -52931,13 +52925,13 @@
         <v>7</v>
       </c>
       <c r="D1597" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1597" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F1597" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H1597">
         <v>1</v>
@@ -52954,13 +52948,13 @@
         <v>7</v>
       </c>
       <c r="D1598" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1598" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F1598" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H1598">
         <v>3</v>
@@ -52977,13 +52971,13 @@
         <v>7</v>
       </c>
       <c r="D1599" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1599" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F1599" s="2" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H1599">
         <v>1</v>
@@ -53000,13 +52994,13 @@
         <v>7</v>
       </c>
       <c r="D1600" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1600" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F1600" s="2" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H1600">
         <v>2</v>
@@ -53023,13 +53017,13 @@
         <v>7</v>
       </c>
       <c r="D1601" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1601" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F1601" s="11" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H1601">
         <v>2</v>
@@ -53046,13 +53040,13 @@
         <v>7</v>
       </c>
       <c r="D1602" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1602" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F1602" s="11" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H1602">
         <v>3</v>
@@ -53069,13 +53063,13 @@
         <v>7</v>
       </c>
       <c r="D1603" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1603" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F1603" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H1603">
         <v>1</v>
@@ -53115,19 +53109,19 @@
         <v>7</v>
       </c>
       <c r="D1605" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1605" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F1605" s="11" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H1605">
         <v>2</v>
       </c>
       <c r="L1605" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="1606" spans="1:12" x14ac:dyDescent="0.2">
@@ -53141,13 +53135,13 @@
         <v>7</v>
       </c>
       <c r="D1606" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1606" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F1606" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H1606">
         <v>1</v>
@@ -53164,13 +53158,13 @@
         <v>7</v>
       </c>
       <c r="D1607" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1607" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F1607" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H1607">
         <v>2</v>
@@ -53187,19 +53181,19 @@
         <v>7</v>
       </c>
       <c r="D1608" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E1608" t="s">
+        <v>945</v>
+      </c>
+      <c r="F1608" s="11" t="s">
+        <v>959</v>
+      </c>
+      <c r="H1608">
+        <v>1</v>
+      </c>
+      <c r="L1608" t="s">
         <v>947</v>
-      </c>
-      <c r="F1608" s="11" t="s">
-        <v>961</v>
-      </c>
-      <c r="H1608">
-        <v>1</v>
-      </c>
-      <c r="L1608" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="1609" spans="1:12" x14ac:dyDescent="0.2">
@@ -53225,10 +53219,10 @@
         <v>1</v>
       </c>
       <c r="I1609" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1609" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="1610" spans="1:12" x14ac:dyDescent="0.2">
@@ -53254,10 +53248,10 @@
         <v>5</v>
       </c>
       <c r="I1610" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="L1610" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="1611" spans="1:12" x14ac:dyDescent="0.2">
@@ -53271,7 +53265,7 @@
         <v>7</v>
       </c>
       <c r="D1611" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="H1611">
         <v>1</v>
@@ -53285,13 +53279,13 @@
         <v>7</v>
       </c>
       <c r="D1612" t="s">
+        <v>950</v>
+      </c>
+      <c r="E1612" t="s">
         <v>952</v>
       </c>
-      <c r="E1612" t="s">
-        <v>954</v>
-      </c>
       <c r="F1612" s="2" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="H1612">
         <v>4</v>
@@ -53305,10 +53299,10 @@
         <v>7</v>
       </c>
       <c r="E1613" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="F1613" s="2" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="H1613">
         <v>1</v>
@@ -53322,13 +53316,13 @@
         <v>7</v>
       </c>
       <c r="D1614" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="E1614" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="F1614" s="2" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="1615" spans="1:12" x14ac:dyDescent="0.2">
@@ -53339,7 +53333,7 @@
         <v>7</v>
       </c>
       <c r="D1615" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="H1615">
         <v>2</v>

</xml_diff>